<commit_message>
Merging after latest SRT meeting
</commit_message>
<xml_diff>
--- a/Translation_to_keyboard_code/LogFiles/Correction factor.xlsx
+++ b/Translation_to_keyboard_code/LogFiles/Correction factor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\Desktop\SRT\Code\Translation_to_keyboard_code\LogFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D953A1-C4A2-488A-BB1E-63C1BF118966}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D7E8E9-1FD4-4089-9423-B20EB671F5C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9E9871BC-E1DB-4C2E-923D-C778FD1FB593}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Calibration:</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>[ 1.303, 1.219, 1.210, 1.194, 1.155, 1.154, 1.134, 1.090, 1.088, 1.155, 1.158, 1.159, 1.183, 1.186, 1.240, 1.373]</t>
+  </si>
+  <si>
+    <t>[ 1.056, 1.020, 0.976, 0.979, 0.948, 0.945, 0.945, 0.939, 0.932, 0.930, 0.941, 0.947, 0.939, 0.941, 1.007, 1.080]</t>
+  </si>
+  <si>
+    <t>[ 1.057, 1.020, 0.976, 0.979, 0.948, 0.945, 0.945, 0.938, 0.931, 0.930, 0.941, 0.947, 0.939, 0.942, 1.007, 1.079]</t>
+  </si>
+  <si>
+    <t>[ 1.057, 1.020, 0.976, 0.979, 0.948, 0.945, 0.945, 0.939, 0.932, 0.929, 0.941, 0.947, 0.939, 0.941, 1.008, 1.080]</t>
+  </si>
+  <si>
+    <t>[ 1.057, 1.020, 0.976, 0.979, 0.948, 0.945, 0.945, 0.938, 0.932, 0.929, 0.941, 0.947, 0.939, 0.941, 1.008, 1.080]</t>
+  </si>
+  <si>
+    <t>[ 1.057, 1.020, 0.976, 0.979, 0.948, 0.945, 0.945, 0.939, 0.932, 0.930, 0.941, 0.947, 0.939, 0.941, 1.008, 1.081]</t>
+  </si>
+  <si>
+    <t>[ 1.057, 1.020, 0.977, 0.979, 0.948, 0.945, 0.945, 0.939, 0.931, 0.930, 0.941, 0.947, 0.939, 0.941, 1.008, 1.080]</t>
   </si>
 </sst>
 </file>
@@ -1584,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E05FF2-12A3-4817-B409-A6C6D8D00CD2}">
-  <dimension ref="A1:BA36"/>
+  <dimension ref="A1:BA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AL36" sqref="AL36"/>
+    <sheetView tabSelected="1" zoomScale="42" workbookViewId="0">
+      <selection activeCell="AL55" sqref="AL55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4755,7 +4773,7 @@
         <v>1.3738571428571427</v>
       </c>
     </row>
-    <row r="33" spans="38:53" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AL33">
         <f>-AL32+AL23</f>
         <v>-0.24997524625835776</v>
@@ -4821,10 +4839,1838 @@
         <v>-0.32068953197264327</v>
       </c>
     </row>
-    <row r="36" spans="38:53" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AL36" t="str">
         <f>_xlfn.CONCAT(AL33,",",AM33,",", AN33, ",",AO33, ",",AP33, ",",AQ33, ",",AR33, ",",AS33, ",",AT33, ",",AU33, ",",AV33, ",",AW33, ",",AX33, ",",AY33, ",",AZ33, ",",BA33 )</f>
         <v>-0.249975246258358,-0.186651358160941,-0.194782136469763,-0.193209159420895,-0.165429551365639,-0.172604021355511,-0.158419862304782,-0.116666462906386,-0.114666462906386,-0.178991290876211,-0.176032592784083,-0.16985812279421,-0.182637730849466,-0.170353565041192,-0.207079929589512,-0.320689531972643</v>
+      </c>
+    </row>
+    <row r="37" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AI37">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="38" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AI38">
+        <f>DEGREES(ATAN(36/108))</f>
+        <v>18.43494882292201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AL39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AL40">
+        <f t="shared" ref="AL40" si="134">AM40+3</f>
+        <v>22.5</v>
+      </c>
+      <c r="AM40">
+        <f t="shared" ref="AM40" si="135">AN40+3</f>
+        <v>19.5</v>
+      </c>
+      <c r="AN40">
+        <f t="shared" ref="AN40" si="136">AO40+3</f>
+        <v>16.5</v>
+      </c>
+      <c r="AO40">
+        <f t="shared" ref="AO40" si="137">AP40+3</f>
+        <v>13.5</v>
+      </c>
+      <c r="AP40">
+        <f t="shared" ref="AP40" si="138">AQ40+3</f>
+        <v>10.5</v>
+      </c>
+      <c r="AQ40">
+        <f t="shared" ref="AQ40" si="139">AR40+3</f>
+        <v>7.5</v>
+      </c>
+      <c r="AR40">
+        <f t="shared" ref="AR40" si="140">AS40+3</f>
+        <v>4.5</v>
+      </c>
+      <c r="AS40">
+        <v>1.5</v>
+      </c>
+      <c r="AT40">
+        <v>1.5</v>
+      </c>
+      <c r="AU40">
+        <f>AT40+3</f>
+        <v>4.5</v>
+      </c>
+      <c r="AV40">
+        <f>AU40+3</f>
+        <v>7.5</v>
+      </c>
+      <c r="AW40">
+        <f t="shared" ref="AW40" si="141">AV40+3</f>
+        <v>10.5</v>
+      </c>
+      <c r="AX40">
+        <f t="shared" ref="AX40" si="142">AW40+3</f>
+        <v>13.5</v>
+      </c>
+      <c r="AY40">
+        <f t="shared" ref="AY40" si="143">AX40+3</f>
+        <v>16.5</v>
+      </c>
+      <c r="AZ40">
+        <f t="shared" ref="AZ40" si="144">AY40+3</f>
+        <v>19.5</v>
+      </c>
+      <c r="BA40">
+        <f t="shared" ref="BA40" si="145">AZ40+3</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="U42" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL42">
+        <f>$B42/COS(RADIANS(AL40))</f>
+        <v>0.83885395522660533</v>
+      </c>
+      <c r="AM42">
+        <f t="shared" ref="AM42:BA42" si="146">$B42/COS(RADIANS(AM40))</f>
+        <v>0.82215774217837267</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" si="146"/>
+        <v>0.80828540737799648</v>
+      </c>
+      <c r="AO42">
+        <f t="shared" si="146"/>
+        <v>0.79702177509053673</v>
+      </c>
+      <c r="AP42">
+        <f t="shared" si="146"/>
+        <v>0.78819845600373073</v>
+      </c>
+      <c r="AQ42">
+        <f t="shared" si="146"/>
+        <v>0.78168744444961835</v>
+      </c>
+      <c r="AR42">
+        <f t="shared" si="146"/>
+        <v>0.77739645382418976</v>
+      </c>
+      <c r="AS42">
+        <f t="shared" si="146"/>
+        <v>0.77526566418042264</v>
+      </c>
+      <c r="AT42">
+        <f t="shared" si="146"/>
+        <v>0.77526566418042264</v>
+      </c>
+      <c r="AU42">
+        <f t="shared" si="146"/>
+        <v>0.77739645382418976</v>
+      </c>
+      <c r="AV42">
+        <f t="shared" si="146"/>
+        <v>0.78168744444961835</v>
+      </c>
+      <c r="AW42">
+        <f t="shared" si="146"/>
+        <v>0.78819845600373073</v>
+      </c>
+      <c r="AX42">
+        <f t="shared" si="146"/>
+        <v>0.79702177509053673</v>
+      </c>
+      <c r="AY42">
+        <f t="shared" si="146"/>
+        <v>0.80828540737799648</v>
+      </c>
+      <c r="AZ42">
+        <f t="shared" si="146"/>
+        <v>0.82215774217837267</v>
+      </c>
+      <c r="BA42">
+        <f t="shared" si="146"/>
+        <v>0.83885395522660533</v>
+      </c>
+    </row>
+    <row r="43" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2">
+        <v>2</v>
+      </c>
+      <c r="G43" s="2">
+        <v>3</v>
+      </c>
+      <c r="H43" s="2">
+        <v>4</v>
+      </c>
+      <c r="I43" s="2">
+        <v>5</v>
+      </c>
+      <c r="J43" s="2">
+        <v>6</v>
+      </c>
+      <c r="K43" s="2">
+        <v>7</v>
+      </c>
+      <c r="L43" s="2">
+        <v>8</v>
+      </c>
+      <c r="M43" s="2">
+        <v>9</v>
+      </c>
+      <c r="N43" s="2">
+        <v>10</v>
+      </c>
+      <c r="O43" s="2">
+        <v>11</v>
+      </c>
+      <c r="P43" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>13</v>
+      </c>
+      <c r="R43" s="2">
+        <v>14</v>
+      </c>
+      <c r="S43" s="2">
+        <v>15</v>
+      </c>
+      <c r="U43" s="2">
+        <v>0</v>
+      </c>
+      <c r="V43" s="2">
+        <v>1</v>
+      </c>
+      <c r="W43" s="2">
+        <v>2</v>
+      </c>
+      <c r="X43" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y43" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z43" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA43" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB43" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC43" s="2">
+        <v>8</v>
+      </c>
+      <c r="AD43" s="2">
+        <v>9</v>
+      </c>
+      <c r="AE43" s="2">
+        <v>10</v>
+      </c>
+      <c r="AF43" s="2">
+        <v>11</v>
+      </c>
+      <c r="AG43" s="2">
+        <v>12</v>
+      </c>
+      <c r="AH43" s="2">
+        <v>13</v>
+      </c>
+      <c r="AI43" s="2">
+        <v>14</v>
+      </c>
+      <c r="AJ43" s="2">
+        <v>15</v>
+      </c>
+      <c r="AL43" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM43" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN43" s="2">
+        <v>2</v>
+      </c>
+      <c r="AO43" s="2">
+        <v>3</v>
+      </c>
+      <c r="AP43" s="2">
+        <v>4</v>
+      </c>
+      <c r="AQ43" s="2">
+        <v>5</v>
+      </c>
+      <c r="AR43" s="2">
+        <v>6</v>
+      </c>
+      <c r="AS43" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT43" s="2">
+        <v>8</v>
+      </c>
+      <c r="AU43" s="2">
+        <v>9</v>
+      </c>
+      <c r="AV43" s="2">
+        <v>10</v>
+      </c>
+      <c r="AW43" s="2">
+        <v>11</v>
+      </c>
+      <c r="AX43" s="2">
+        <v>12</v>
+      </c>
+      <c r="AY43" s="2">
+        <v>13</v>
+      </c>
+      <c r="AZ43" s="2">
+        <v>14</v>
+      </c>
+      <c r="BA43" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <f>FIND(",",$A44,D44+1)</f>
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <f t="shared" ref="F44:F50" si="147">FIND(",",$A44,E44+1)</f>
+        <v>15</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44:G50" si="148">FIND(",",$A44,F44+1)</f>
+        <v>22</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ref="H44:H50" si="149">FIND(",",$A44,G44+1)</f>
+        <v>29</v>
+      </c>
+      <c r="I44">
+        <f t="shared" ref="I44:I50" si="150">FIND(",",$A44,H44+1)</f>
+        <v>36</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ref="J44:J50" si="151">FIND(",",$A44,I44+1)</f>
+        <v>43</v>
+      </c>
+      <c r="K44">
+        <f t="shared" ref="K44:K50" si="152">FIND(",",$A44,J44+1)</f>
+        <v>50</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ref="L44:L50" si="153">FIND(",",$A44,K44+1)</f>
+        <v>57</v>
+      </c>
+      <c r="M44">
+        <f t="shared" ref="M44:M50" si="154">FIND(",",$A44,L44+1)</f>
+        <v>64</v>
+      </c>
+      <c r="N44">
+        <f t="shared" ref="N44:N50" si="155">FIND(",",$A44,M44+1)</f>
+        <v>71</v>
+      </c>
+      <c r="O44">
+        <f t="shared" ref="O44:O50" si="156">FIND(",",$A44,N44+1)</f>
+        <v>78</v>
+      </c>
+      <c r="P44">
+        <f t="shared" ref="P44:P50" si="157">FIND(",",$A44,O44+1)</f>
+        <v>85</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" ref="Q44:Q50" si="158">FIND(",",$A44,P44+1)</f>
+        <v>92</v>
+      </c>
+      <c r="R44">
+        <f t="shared" ref="R44:R50" si="159">FIND(",",$A44,Q44+1)</f>
+        <v>99</v>
+      </c>
+      <c r="S44">
+        <f t="shared" ref="S44:S50" si="160">FIND(",",$A44,R44+1)</f>
+        <v>106</v>
+      </c>
+      <c r="U44" t="str">
+        <f>MID($A44,D44+1,E44-D44-1)</f>
+        <v xml:space="preserve"> 1.056</v>
+      </c>
+      <c r="V44" t="str">
+        <f t="shared" ref="V44:V50" si="161">MID($A44,E44+1,F44-E44-1)</f>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W44" t="str">
+        <f t="shared" ref="W44:W50" si="162">MID($A44,F44+1,G44-F44-1)</f>
+        <v xml:space="preserve"> 0.976</v>
+      </c>
+      <c r="X44" t="str">
+        <f t="shared" ref="X44:X50" si="163">MID($A44,G44+1,H44-G44-1)</f>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y44" t="str">
+        <f t="shared" ref="Y44:Y50" si="164">MID($A44,H44+1,I44-H44-1)</f>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z44" t="str">
+        <f t="shared" ref="Z44:Z50" si="165">MID($A44,I44+1,J44-I44-1)</f>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA44" t="str">
+        <f t="shared" ref="AA44:AA50" si="166">MID($A44,J44+1,K44-J44-1)</f>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB44" t="str">
+        <f t="shared" ref="AB44:AB50" si="167">MID($A44,K44+1,L44-K44-1)</f>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AC44" t="str">
+        <f t="shared" ref="AC44:AC50" si="168">MID($A44,L44+1,M44-L44-1)</f>
+        <v xml:space="preserve"> 0.932</v>
+      </c>
+      <c r="AD44" t="str">
+        <f t="shared" ref="AD44:AD50" si="169">MID($A44,M44+1,N44-M44-1)</f>
+        <v xml:space="preserve"> 0.930</v>
+      </c>
+      <c r="AE44" t="str">
+        <f t="shared" ref="AE44:AE50" si="170">MID($A44,N44+1,O44-N44-1)</f>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF44" t="str">
+        <f t="shared" ref="AF44:AF50" si="171">MID($A44,O44+1,P44-O44-1)</f>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG44" t="str">
+        <f t="shared" ref="AG44:AG50" si="172">MID($A44,P44+1,Q44-P44-1)</f>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH44" t="str">
+        <f t="shared" ref="AH44:AH50" si="173">MID($A44,Q44+1,R44-Q44-1)</f>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AI44" t="str">
+        <f t="shared" ref="AI44:AI50" si="174">MID($A44,R44+1,S44-R44-1)</f>
+        <v xml:space="preserve"> 1.007</v>
+      </c>
+      <c r="AJ44" t="str">
+        <f>MID($A44,S44+1,6)</f>
+        <v xml:space="preserve"> 1.080</v>
+      </c>
+      <c r="AL44">
+        <f>_xlfn.NUMBERVALUE(U44)</f>
+        <v>1.056</v>
+      </c>
+      <c r="AM44">
+        <f t="shared" ref="AM44:AM50" si="175">_xlfn.NUMBERVALUE(V44)</f>
+        <v>1.02</v>
+      </c>
+      <c r="AN44">
+        <f t="shared" ref="AN44:AN50" si="176">_xlfn.NUMBERVALUE(W44)</f>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO44">
+        <f t="shared" ref="AO44:AO50" si="177">_xlfn.NUMBERVALUE(X44)</f>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP44">
+        <f t="shared" ref="AP44:AP50" si="178">_xlfn.NUMBERVALUE(Y44)</f>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ44">
+        <f t="shared" ref="AQ44:AQ50" si="179">_xlfn.NUMBERVALUE(Z44)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR44">
+        <f t="shared" ref="AR44:AR50" si="180">_xlfn.NUMBERVALUE(AA44)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS44">
+        <f t="shared" ref="AS44:AS50" si="181">_xlfn.NUMBERVALUE(AB44)</f>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AT44">
+        <f t="shared" ref="AT44:AT50" si="182">_xlfn.NUMBERVALUE(AC44)</f>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AU44">
+        <f t="shared" ref="AU44:AU50" si="183">_xlfn.NUMBERVALUE(AD44)</f>
+        <v>0.93</v>
+      </c>
+      <c r="AV44">
+        <f t="shared" ref="AV44:AV50" si="184">_xlfn.NUMBERVALUE(AE44)</f>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW44">
+        <f t="shared" ref="AW44:AW50" si="185">_xlfn.NUMBERVALUE(AF44)</f>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX44">
+        <f t="shared" ref="AX44:AX50" si="186">_xlfn.NUMBERVALUE(AG44)</f>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY44">
+        <f t="shared" ref="AY44:AY50" si="187">_xlfn.NUMBERVALUE(AH44)</f>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AZ44">
+        <f t="shared" ref="AZ44:AZ50" si="188">_xlfn.NUMBERVALUE(AI44)</f>
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="BA44">
+        <f t="shared" ref="BA44:BA50" si="189">_xlfn.NUMBERVALUE(AJ44)</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="45" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ref="E45:E50" si="190">FIND(",",$A45,D45+1)</f>
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="147"/>
+        <v>15</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="148"/>
+        <v>22</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="149"/>
+        <v>29</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="150"/>
+        <v>36</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="151"/>
+        <v>43</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="152"/>
+        <v>50</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="153"/>
+        <v>57</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="154"/>
+        <v>64</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="155"/>
+        <v>71</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="156"/>
+        <v>78</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="157"/>
+        <v>85</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="158"/>
+        <v>92</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="159"/>
+        <v>99</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="U45" t="str">
+        <f t="shared" ref="U45:U50" si="191">MID($A45,D45+1,E45-D45-1)</f>
+        <v xml:space="preserve"> 1.057</v>
+      </c>
+      <c r="V45" t="str">
+        <f t="shared" si="161"/>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W45" t="str">
+        <f t="shared" si="162"/>
+        <v xml:space="preserve"> 0.976</v>
+      </c>
+      <c r="X45" t="str">
+        <f t="shared" si="163"/>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y45" t="str">
+        <f t="shared" si="164"/>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z45" t="str">
+        <f t="shared" si="165"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA45" t="str">
+        <f t="shared" si="166"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB45" t="str">
+        <f t="shared" si="167"/>
+        <v xml:space="preserve"> 0.938</v>
+      </c>
+      <c r="AC45" t="str">
+        <f t="shared" si="168"/>
+        <v xml:space="preserve"> 0.931</v>
+      </c>
+      <c r="AD45" t="str">
+        <f t="shared" si="169"/>
+        <v xml:space="preserve"> 0.930</v>
+      </c>
+      <c r="AE45" t="str">
+        <f t="shared" si="170"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF45" t="str">
+        <f t="shared" si="171"/>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG45" t="str">
+        <f t="shared" si="172"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH45" t="str">
+        <f t="shared" si="173"/>
+        <v xml:space="preserve"> 0.942</v>
+      </c>
+      <c r="AI45" t="str">
+        <f t="shared" si="174"/>
+        <v xml:space="preserve"> 1.007</v>
+      </c>
+      <c r="AJ45" t="str">
+        <f t="shared" ref="AJ45:AJ50" si="192">MID($A45,S45+1,6)</f>
+        <v xml:space="preserve"> 1.079</v>
+      </c>
+      <c r="AL45">
+        <f t="shared" ref="AL45:AL50" si="193">_xlfn.NUMBERVALUE(U45)</f>
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="AM45">
+        <f t="shared" si="175"/>
+        <v>1.02</v>
+      </c>
+      <c r="AN45">
+        <f t="shared" si="176"/>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO45">
+        <f t="shared" si="177"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP45">
+        <f t="shared" si="178"/>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ45">
+        <f t="shared" si="179"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR45">
+        <f t="shared" si="180"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS45">
+        <f t="shared" si="181"/>
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="AT45">
+        <f t="shared" si="182"/>
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="AU45">
+        <f t="shared" si="183"/>
+        <v>0.93</v>
+      </c>
+      <c r="AV45">
+        <f t="shared" si="184"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW45">
+        <f t="shared" si="185"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX45">
+        <f t="shared" si="186"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY45">
+        <f t="shared" si="187"/>
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="AZ45">
+        <f t="shared" si="188"/>
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="BA45">
+        <f t="shared" si="189"/>
+        <v>1.079</v>
+      </c>
+    </row>
+    <row r="46" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="190"/>
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="147"/>
+        <v>15</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="148"/>
+        <v>22</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="149"/>
+        <v>29</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="150"/>
+        <v>36</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="151"/>
+        <v>43</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="152"/>
+        <v>50</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="153"/>
+        <v>57</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="154"/>
+        <v>64</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="155"/>
+        <v>71</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="156"/>
+        <v>78</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="157"/>
+        <v>85</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="158"/>
+        <v>92</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="159"/>
+        <v>99</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="U46" t="str">
+        <f t="shared" si="191"/>
+        <v xml:space="preserve"> 1.057</v>
+      </c>
+      <c r="V46" t="str">
+        <f t="shared" si="161"/>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W46" t="str">
+        <f t="shared" si="162"/>
+        <v xml:space="preserve"> 0.976</v>
+      </c>
+      <c r="X46" t="str">
+        <f t="shared" si="163"/>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y46" t="str">
+        <f t="shared" si="164"/>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z46" t="str">
+        <f t="shared" si="165"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA46" t="str">
+        <f t="shared" si="166"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB46" t="str">
+        <f t="shared" si="167"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AC46" t="str">
+        <f t="shared" si="168"/>
+        <v xml:space="preserve"> 0.932</v>
+      </c>
+      <c r="AD46" t="str">
+        <f t="shared" si="169"/>
+        <v xml:space="preserve"> 0.929</v>
+      </c>
+      <c r="AE46" t="str">
+        <f t="shared" si="170"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF46" t="str">
+        <f t="shared" si="171"/>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG46" t="str">
+        <f t="shared" si="172"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH46" t="str">
+        <f t="shared" si="173"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AI46" t="str">
+        <f t="shared" si="174"/>
+        <v xml:space="preserve"> 1.008</v>
+      </c>
+      <c r="AJ46" t="str">
+        <f t="shared" si="192"/>
+        <v xml:space="preserve"> 1.080</v>
+      </c>
+      <c r="AL46">
+        <f t="shared" si="193"/>
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="AM46">
+        <f t="shared" si="175"/>
+        <v>1.02</v>
+      </c>
+      <c r="AN46">
+        <f t="shared" si="176"/>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO46">
+        <f t="shared" si="177"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP46">
+        <f t="shared" si="178"/>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ46">
+        <f t="shared" si="179"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR46">
+        <f t="shared" si="180"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS46">
+        <f t="shared" si="181"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AT46">
+        <f t="shared" si="182"/>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AU46">
+        <f t="shared" si="183"/>
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="AV46">
+        <f t="shared" si="184"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW46">
+        <f t="shared" si="185"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX46">
+        <f t="shared" si="186"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY46">
+        <f t="shared" si="187"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AZ46">
+        <f t="shared" si="188"/>
+        <v>1.008</v>
+      </c>
+      <c r="BA46">
+        <f t="shared" si="189"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="47" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="190"/>
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="147"/>
+        <v>15</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="148"/>
+        <v>22</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="149"/>
+        <v>29</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="150"/>
+        <v>36</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="151"/>
+        <v>43</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="152"/>
+        <v>50</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="153"/>
+        <v>57</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="154"/>
+        <v>64</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="155"/>
+        <v>71</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="156"/>
+        <v>78</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="157"/>
+        <v>85</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="158"/>
+        <v>92</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="159"/>
+        <v>99</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="U47" t="str">
+        <f t="shared" si="191"/>
+        <v xml:space="preserve"> 1.057</v>
+      </c>
+      <c r="V47" t="str">
+        <f t="shared" si="161"/>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W47" t="str">
+        <f t="shared" si="162"/>
+        <v xml:space="preserve"> 0.976</v>
+      </c>
+      <c r="X47" t="str">
+        <f t="shared" si="163"/>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y47" t="str">
+        <f t="shared" si="164"/>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z47" t="str">
+        <f t="shared" si="165"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA47" t="str">
+        <f t="shared" si="166"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB47" t="str">
+        <f t="shared" si="167"/>
+        <v xml:space="preserve"> 0.938</v>
+      </c>
+      <c r="AC47" t="str">
+        <f t="shared" si="168"/>
+        <v xml:space="preserve"> 0.932</v>
+      </c>
+      <c r="AD47" t="str">
+        <f t="shared" si="169"/>
+        <v xml:space="preserve"> 0.929</v>
+      </c>
+      <c r="AE47" t="str">
+        <f t="shared" si="170"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF47" t="str">
+        <f t="shared" si="171"/>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG47" t="str">
+        <f t="shared" si="172"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH47" t="str">
+        <f t="shared" si="173"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AI47" t="str">
+        <f t="shared" si="174"/>
+        <v xml:space="preserve"> 1.008</v>
+      </c>
+      <c r="AJ47" t="str">
+        <f t="shared" si="192"/>
+        <v xml:space="preserve"> 1.080</v>
+      </c>
+      <c r="AL47">
+        <f t="shared" si="193"/>
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="AM47">
+        <f t="shared" si="175"/>
+        <v>1.02</v>
+      </c>
+      <c r="AN47">
+        <f t="shared" si="176"/>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO47">
+        <f t="shared" si="177"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP47">
+        <f t="shared" si="178"/>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ47">
+        <f t="shared" si="179"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR47">
+        <f t="shared" si="180"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS47">
+        <f t="shared" si="181"/>
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="AT47">
+        <f t="shared" si="182"/>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AU47">
+        <f t="shared" si="183"/>
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="AV47">
+        <f t="shared" si="184"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW47">
+        <f t="shared" si="185"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX47">
+        <f t="shared" si="186"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY47">
+        <f t="shared" si="187"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AZ47">
+        <f t="shared" si="188"/>
+        <v>1.008</v>
+      </c>
+      <c r="BA47">
+        <f t="shared" si="189"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="48" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="190"/>
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="147"/>
+        <v>15</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="148"/>
+        <v>22</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="149"/>
+        <v>29</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="150"/>
+        <v>36</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="151"/>
+        <v>43</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="152"/>
+        <v>50</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="153"/>
+        <v>57</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="154"/>
+        <v>64</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="155"/>
+        <v>71</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="156"/>
+        <v>78</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="157"/>
+        <v>85</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="158"/>
+        <v>92</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="159"/>
+        <v>99</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="U48" t="str">
+        <f t="shared" si="191"/>
+        <v xml:space="preserve"> 1.057</v>
+      </c>
+      <c r="V48" t="str">
+        <f t="shared" si="161"/>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W48" t="str">
+        <f t="shared" si="162"/>
+        <v xml:space="preserve"> 0.976</v>
+      </c>
+      <c r="X48" t="str">
+        <f t="shared" si="163"/>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y48" t="str">
+        <f t="shared" si="164"/>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z48" t="str">
+        <f t="shared" si="165"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA48" t="str">
+        <f t="shared" si="166"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB48" t="str">
+        <f t="shared" si="167"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AC48" t="str">
+        <f t="shared" si="168"/>
+        <v xml:space="preserve"> 0.932</v>
+      </c>
+      <c r="AD48" t="str">
+        <f t="shared" si="169"/>
+        <v xml:space="preserve"> 0.930</v>
+      </c>
+      <c r="AE48" t="str">
+        <f t="shared" si="170"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF48" t="str">
+        <f t="shared" si="171"/>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG48" t="str">
+        <f t="shared" si="172"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH48" t="str">
+        <f t="shared" si="173"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AI48" t="str">
+        <f t="shared" si="174"/>
+        <v xml:space="preserve"> 1.008</v>
+      </c>
+      <c r="AJ48" t="str">
+        <f t="shared" si="192"/>
+        <v xml:space="preserve"> 1.081</v>
+      </c>
+      <c r="AL48">
+        <f t="shared" si="193"/>
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="AM48">
+        <f t="shared" si="175"/>
+        <v>1.02</v>
+      </c>
+      <c r="AN48">
+        <f t="shared" si="176"/>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO48">
+        <f t="shared" si="177"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP48">
+        <f t="shared" si="178"/>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ48">
+        <f t="shared" si="179"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR48">
+        <f t="shared" si="180"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS48">
+        <f t="shared" si="181"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AT48">
+        <f t="shared" si="182"/>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AU48">
+        <f t="shared" si="183"/>
+        <v>0.93</v>
+      </c>
+      <c r="AV48">
+        <f t="shared" si="184"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW48">
+        <f t="shared" si="185"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX48">
+        <f t="shared" si="186"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY48">
+        <f t="shared" si="187"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AZ48">
+        <f t="shared" si="188"/>
+        <v>1.008</v>
+      </c>
+      <c r="BA48">
+        <f t="shared" si="189"/>
+        <v>1.081</v>
+      </c>
+    </row>
+    <row r="49" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="190"/>
+        <v>8</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="147"/>
+        <v>15</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="148"/>
+        <v>22</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="149"/>
+        <v>29</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="150"/>
+        <v>36</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="151"/>
+        <v>43</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="152"/>
+        <v>50</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="153"/>
+        <v>57</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="154"/>
+        <v>64</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="155"/>
+        <v>71</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="156"/>
+        <v>78</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="157"/>
+        <v>85</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="158"/>
+        <v>92</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="159"/>
+        <v>99</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="U49" t="str">
+        <f t="shared" si="191"/>
+        <v xml:space="preserve"> 1.057</v>
+      </c>
+      <c r="V49" t="str">
+        <f t="shared" si="161"/>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W49" t="str">
+        <f t="shared" si="162"/>
+        <v xml:space="preserve"> 0.976</v>
+      </c>
+      <c r="X49" t="str">
+        <f t="shared" si="163"/>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y49" t="str">
+        <f t="shared" si="164"/>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z49" t="str">
+        <f t="shared" si="165"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA49" t="str">
+        <f t="shared" si="166"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB49" t="str">
+        <f t="shared" si="167"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AC49" t="str">
+        <f t="shared" si="168"/>
+        <v xml:space="preserve"> 0.932</v>
+      </c>
+      <c r="AD49" t="str">
+        <f t="shared" si="169"/>
+        <v xml:space="preserve"> 0.929</v>
+      </c>
+      <c r="AE49" t="str">
+        <f t="shared" si="170"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF49" t="str">
+        <f t="shared" si="171"/>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG49" t="str">
+        <f t="shared" si="172"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH49" t="str">
+        <f t="shared" si="173"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AI49" t="str">
+        <f t="shared" si="174"/>
+        <v xml:space="preserve"> 1.008</v>
+      </c>
+      <c r="AJ49" t="str">
+        <f t="shared" si="192"/>
+        <v xml:space="preserve"> 1.080</v>
+      </c>
+      <c r="AL49">
+        <f t="shared" si="193"/>
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="AM49">
+        <f t="shared" si="175"/>
+        <v>1.02</v>
+      </c>
+      <c r="AN49">
+        <f t="shared" si="176"/>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO49">
+        <f t="shared" si="177"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP49">
+        <f t="shared" si="178"/>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ49">
+        <f t="shared" si="179"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR49">
+        <f t="shared" si="180"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS49">
+        <f t="shared" si="181"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AT49">
+        <f t="shared" si="182"/>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="AU49">
+        <f t="shared" si="183"/>
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="AV49">
+        <f t="shared" si="184"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW49">
+        <f t="shared" si="185"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX49">
+        <f t="shared" si="186"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY49">
+        <f t="shared" si="187"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AZ49">
+        <f t="shared" si="188"/>
+        <v>1.008</v>
+      </c>
+      <c r="BA49">
+        <f t="shared" si="189"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="190"/>
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="147"/>
+        <v>15</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="148"/>
+        <v>22</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="149"/>
+        <v>29</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="150"/>
+        <v>36</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="151"/>
+        <v>43</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="152"/>
+        <v>50</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="153"/>
+        <v>57</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="154"/>
+        <v>64</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="155"/>
+        <v>71</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="156"/>
+        <v>78</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="157"/>
+        <v>85</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="158"/>
+        <v>92</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="159"/>
+        <v>99</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="U50" t="str">
+        <f t="shared" si="191"/>
+        <v xml:space="preserve"> 1.057</v>
+      </c>
+      <c r="V50" t="str">
+        <f t="shared" si="161"/>
+        <v xml:space="preserve"> 1.020</v>
+      </c>
+      <c r="W50" t="str">
+        <f t="shared" si="162"/>
+        <v xml:space="preserve"> 0.977</v>
+      </c>
+      <c r="X50" t="str">
+        <f t="shared" si="163"/>
+        <v xml:space="preserve"> 0.979</v>
+      </c>
+      <c r="Y50" t="str">
+        <f t="shared" si="164"/>
+        <v xml:space="preserve"> 0.948</v>
+      </c>
+      <c r="Z50" t="str">
+        <f t="shared" si="165"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AA50" t="str">
+        <f t="shared" si="166"/>
+        <v xml:space="preserve"> 0.945</v>
+      </c>
+      <c r="AB50" t="str">
+        <f t="shared" si="167"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AC50" t="str">
+        <f t="shared" si="168"/>
+        <v xml:space="preserve"> 0.931</v>
+      </c>
+      <c r="AD50" t="str">
+        <f t="shared" si="169"/>
+        <v xml:space="preserve"> 0.930</v>
+      </c>
+      <c r="AE50" t="str">
+        <f t="shared" si="170"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AF50" t="str">
+        <f t="shared" si="171"/>
+        <v xml:space="preserve"> 0.947</v>
+      </c>
+      <c r="AG50" t="str">
+        <f t="shared" si="172"/>
+        <v xml:space="preserve"> 0.939</v>
+      </c>
+      <c r="AH50" t="str">
+        <f t="shared" si="173"/>
+        <v xml:space="preserve"> 0.941</v>
+      </c>
+      <c r="AI50" t="str">
+        <f t="shared" si="174"/>
+        <v xml:space="preserve"> 1.008</v>
+      </c>
+      <c r="AJ50" t="str">
+        <f t="shared" si="192"/>
+        <v xml:space="preserve"> 1.080</v>
+      </c>
+      <c r="AL50">
+        <f t="shared" si="193"/>
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="AM50">
+        <f t="shared" si="175"/>
+        <v>1.02</v>
+      </c>
+      <c r="AN50">
+        <f t="shared" si="176"/>
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="AO50">
+        <f t="shared" si="177"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP50">
+        <f t="shared" si="178"/>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="AQ50">
+        <f t="shared" si="179"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AR50">
+        <f t="shared" si="180"/>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AS50">
+        <f t="shared" si="181"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AT50">
+        <f t="shared" si="182"/>
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="AU50">
+        <f t="shared" si="183"/>
+        <v>0.93</v>
+      </c>
+      <c r="AV50">
+        <f t="shared" si="184"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW50">
+        <f t="shared" si="185"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX50">
+        <f t="shared" si="186"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY50">
+        <f t="shared" si="187"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AZ50">
+        <f t="shared" si="188"/>
+        <v>1.008</v>
+      </c>
+      <c r="BA50">
+        <f t="shared" si="189"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="51" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AL51">
+        <f>AVERAGE(AL44:AL50)</f>
+        <v>1.0568571428571432</v>
+      </c>
+      <c r="AM51">
+        <f t="shared" ref="AM51:BA51" si="194">AVERAGE(AM44:AM50)</f>
+        <v>1.0199999999999998</v>
+      </c>
+      <c r="AN51">
+        <f t="shared" si="194"/>
+        <v>0.9761428571428572</v>
+      </c>
+      <c r="AO51">
+        <f t="shared" si="194"/>
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="AP51">
+        <f t="shared" si="194"/>
+        <v>0.94800000000000018</v>
+      </c>
+      <c r="AQ51">
+        <f t="shared" si="194"/>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="AR51">
+        <f t="shared" si="194"/>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="AS51">
+        <f t="shared" si="194"/>
+        <v>0.93871428571428572</v>
+      </c>
+      <c r="AT51">
+        <f t="shared" si="194"/>
+        <v>0.93171428571428572</v>
+      </c>
+      <c r="AU51">
+        <f t="shared" si="194"/>
+        <v>0.92957142857142849</v>
+      </c>
+      <c r="AV51">
+        <f t="shared" si="194"/>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="AW51">
+        <f t="shared" si="194"/>
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="AX51">
+        <f t="shared" si="194"/>
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AY51">
+        <f t="shared" si="194"/>
+        <v>0.94114285714285706</v>
+      </c>
+      <c r="AZ51">
+        <f t="shared" si="194"/>
+        <v>1.0077142857142856</v>
+      </c>
+      <c r="BA51">
+        <f t="shared" si="194"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="52" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AL52">
+        <f>-AL51+AL42</f>
+        <v>-0.21800318763053783</v>
+      </c>
+      <c r="AM52">
+        <f t="shared" ref="AM52:BA52" si="195">-AM51+AM42</f>
+        <v>-0.19784225782162712</v>
+      </c>
+      <c r="AN52">
+        <f t="shared" si="195"/>
+        <v>-0.16785744976486072</v>
+      </c>
+      <c r="AO52">
+        <f t="shared" si="195"/>
+        <v>-0.18197822490946325</v>
+      </c>
+      <c r="AP52">
+        <f t="shared" si="195"/>
+        <v>-0.15980154399626945</v>
+      </c>
+      <c r="AQ52">
+        <f t="shared" si="195"/>
+        <v>-0.16331255555038171</v>
+      </c>
+      <c r="AR52">
+        <f t="shared" si="195"/>
+        <v>-0.1676035461758103</v>
+      </c>
+      <c r="AS52">
+        <f t="shared" si="195"/>
+        <v>-0.16344862153386308</v>
+      </c>
+      <c r="AT52">
+        <f t="shared" si="195"/>
+        <v>-0.15644862153386307</v>
+      </c>
+      <c r="AU52">
+        <f t="shared" si="195"/>
+        <v>-0.15217497474723873</v>
+      </c>
+      <c r="AV52">
+        <f t="shared" si="195"/>
+        <v>-0.1593125555503816</v>
+      </c>
+      <c r="AW52">
+        <f t="shared" si="195"/>
+        <v>-0.15880154399626922</v>
+      </c>
+      <c r="AX52">
+        <f t="shared" si="195"/>
+        <v>-0.14197822490946321</v>
+      </c>
+      <c r="AY52">
+        <f t="shared" si="195"/>
+        <v>-0.13285744976486058</v>
+      </c>
+      <c r="AZ52">
+        <f t="shared" si="195"/>
+        <v>-0.18555654353591289</v>
+      </c>
+      <c r="BA52">
+        <f t="shared" si="195"/>
+        <v>-0.24114604477339474</v>
+      </c>
+    </row>
+    <row r="55" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AL55" t="str">
+        <f>_xlfn.CONCAT(AL52,",",AM52,",", AN52, ",",AO52, ",",AP52, ",",AQ52, ",",AR52, ",",AS52, ",",AT52, ",",AU52, ",",AV52, ",",AW52, ",",AX52, ",",AY52, ",",AZ52, ",",BA52 )</f>
+        <v>-0.218003187630538,-0.197842257821627,-0.167857449764861,-0.181978224909463,-0.159801543996269,-0.163312555550382,-0.16760354617581,-0.163448621533863,-0.156448621533863,-0.152174974747239,-0.159312555550382,-0.158801543996269,-0.141978224909463,-0.132857449764861,-0.185556543535913,-0.241146044773395</v>
+      </c>
+    </row>
+    <row r="56" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AL56" t="str">
+        <f>_xlfn.CONCAT(AL42,",",AM42,",", AN42, ",",AO42, ",",AP42, ",",AQ42, ",",AR42, ",",AS42, ",",AT42, ",",AU42, ",",AV42, ",",AW42, ",",AX42, ",",AY42, ",",AZ42, ",",BA42 )</f>
+        <v>0.838853955226605,0.822157742178373,0.808285407377996,0.797021775090537,0.788198456003731,0.781687444449618,0.77739645382419,0.775265664180423,0.775265664180423,0.77739645382419,0.781687444449618,0.788198456003731,0.797021775090537,0.808285407377996,0.822157742178373,0.838853955226605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>